<commit_message>
update the example data for connectivity
</commit_message>
<xml_diff>
--- a/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName1/covariates/GroupName1_covariates.xlsx
+++ b/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName1/covariates/GroupName1_covariates.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
   <si>
     <t>edu</t>
@@ -312,7 +327,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
@@ -320,13 +335,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>53</v>
       </c>
       <c r="D2" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -334,13 +349,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -348,13 +363,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -362,13 +377,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -379,10 +394,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -390,13 +405,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -404,13 +419,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -418,13 +433,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -432,13 +447,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -446,13 +461,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -460,13 +475,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D12" s="0">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -474,13 +489,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D13" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -488,13 +503,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -502,13 +517,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D15" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -516,13 +531,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D16" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -530,13 +545,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D17" s="0">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -544,13 +559,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18" s="0">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -558,13 +573,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -572,13 +587,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -586,13 +601,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -603,10 +618,10 @@
         <v>62</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="0">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
@@ -614,13 +629,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
@@ -628,13 +643,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="0">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D24" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -642,13 +657,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="0">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D25" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -656,13 +671,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="0">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="0">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -670,13 +685,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="0">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="0">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
@@ -684,10 +699,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="0">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="0">
         <v>9</v>
@@ -698,10 +713,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="0">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="0">
         <v>5</v>
@@ -712,13 +727,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="0">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="0">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -726,13 +741,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="0">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>67</v>
       </c>
       <c r="D31" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -740,13 +755,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D32" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
@@ -754,13 +769,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D33" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
@@ -768,13 +783,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="0">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D34" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
@@ -782,13 +797,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D35" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
@@ -796,10 +811,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="0">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D36" s="0">
         <v>13</v>
@@ -810,13 +825,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="0">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D37" s="0">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
@@ -824,13 +839,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D38" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -838,13 +853,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D39" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40">
@@ -852,10 +867,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="0">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D40" s="0">
         <v>10</v>
@@ -866,13 +881,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="0">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D41" s="0">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -880,13 +895,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="0">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D42" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -894,13 +909,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="0">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D43" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
@@ -908,13 +923,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="0">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D44" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
@@ -922,13 +937,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="0">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D45" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46">
@@ -936,13 +951,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="0">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D46" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -950,13 +965,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D47" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
@@ -964,10 +979,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="0">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D48" s="0">
         <v>5</v>
@@ -978,13 +993,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="0">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D49" s="0">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -992,13 +1007,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="0">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D50" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
@@ -1006,13 +1021,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="0">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D51" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>